<commit_message>
Update CHANGELOG and other small changes to code
</commit_message>
<xml_diff>
--- a/home/tests/import-export-data/high_inflection_invalid_format.xlsx
+++ b/home/tests/import-export-data/high_inflection_invalid_format.xlsx
@@ -142,9 +142,6 @@
     <t xml:space="preserve">mnch_onboarding_dma_results_high</t>
   </si>
   <si>
-    <t xml:space="preserve">5,0</t>
-  </si>
-  <si>
     <t xml:space="preserve">mnch_onboarding_dma_results_medium</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t xml:space="preserve">DMA_Form_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,0</t>
   </si>
   <si>
     <t xml:space="preserve">Here’s a next one:
@@ -506,10 +506,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -617,43 +617,43 @@
       <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="H2" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
@@ -673,7 +673,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>20</v>
@@ -692,39 +692,39 @@
         <v>5</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K3" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -744,7 +744,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>20</v>
@@ -763,39 +763,39 @@
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K4" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
@@ -815,7 +815,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>20</v>
@@ -830,36 +830,36 @@
       <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="11" t="n">
-        <v>5</v>
+      <c r="F5" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>43</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
@@ -905,32 +905,32 @@
         <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3" t="s">

</xml_diff>